<commit_message>
Introduces sort sort key functions in display.php
</commit_message>
<xml_diff>
--- a/Documentation/ManagerView/ManagerView.xlsx
+++ b/Documentation/ManagerView/ManagerView.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CentRes\Documentation\ManagerView\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C26016-AD66-45EC-9025-92B78CB6B288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085D085A-A72F-4E2E-8E70-9F163B90D9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C5EF8A08-DD46-4887-AEB9-AF506434A2C8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>Menu Item</t>
   </si>
@@ -112,12 +112,6 @@
   </si>
   <si>
     <t>&lt;&lt;&lt;&lt;&lt;</t>
-  </si>
-  <si>
-    <t>setVar("sortKey1", "category ASC");</t>
-  </si>
-  <si>
-    <t>setVar("sortKey2", "requests DESC");</t>
   </si>
   <si>
     <t>asdfasfdf</t>
@@ -361,6 +355,12 @@
   </si>
   <si>
     <t>② Requests ▼</t>
+  </si>
+  <si>
+    <t>toggleSortKey("myTableId", "MenuItems.requests");</t>
+  </si>
+  <si>
+    <t>toggleSortKey("myTableId", "MenuCategories.name");  //toggle rotates through unsorted, sorted ASC, sorted DESC</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -988,11 +988,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1175,51 +1199,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1241,8 +1222,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1753,7 +1783,7 @@
   <dimension ref="A1:AE46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -1765,7 +1795,7 @@
     <col min="5" max="5" width="18.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.7265625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.7265625" style="1"/>
-    <col min="8" max="8" width="52.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="133.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="1.81640625" style="1" customWidth="1"/>
     <col min="10" max="11" width="8.7265625" style="1"/>
     <col min="12" max="12" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
@@ -1786,14 +1816,14 @@
   <sheetData>
     <row r="1" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:31" ht="31" x14ac:dyDescent="0.35">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:31" ht="9.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
@@ -1802,15 +1832,15 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="U3" s="79" t="s">
+      <c r="U3" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="80"/>
-      <c r="W3" s="80"/>
-      <c r="X3" s="80"/>
-      <c r="Y3" s="80"/>
-      <c r="Z3" s="81"/>
-      <c r="AA3" s="81"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="67"/>
+      <c r="Z3" s="68"/>
+      <c r="AA3" s="68"/>
     </row>
     <row r="4" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
@@ -1822,7 +1852,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>13</v>
@@ -1907,11 +1937,11 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="82" t="s">
+      <c r="G9" s="69" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>15</v>
@@ -1926,18 +1956,18 @@
         <v>0</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="33" t="s">
-        <v>26</v>
+      <c r="G10" s="70"/>
+      <c r="H10" s="86" t="s">
+        <v>86</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>16</v>
@@ -1946,21 +1976,21 @@
       <c r="M10" s="16"/>
       <c r="N10" s="16"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="30"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="8"/>
       <c r="F11" s="3"/>
-      <c r="H11" s="1" t="s">
-        <v>22</v>
+      <c r="H11" s="87" t="s">
+        <v>86</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="10"/>
@@ -1968,48 +1998,48 @@
       <c r="E12" s="8"/>
       <c r="F12" s="3"/>
       <c r="H12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y12" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z12" s="66"/>
-      <c r="AA12" s="66"/>
-      <c r="AB12" s="66"/>
-      <c r="AC12" s="66"/>
-      <c r="AD12" s="66"/>
-      <c r="AE12" s="66"/>
+      <c r="Y12" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z12" s="75"/>
+      <c r="AA12" s="75"/>
+      <c r="AB12" s="75"/>
+      <c r="AC12" s="75"/>
+      <c r="AD12" s="75"/>
+      <c r="AE12" s="75"/>
     </row>
     <row r="13" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
       <c r="B13" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="22">
         <v>17</v>
       </c>
       <c r="F13" s="3"/>
-      <c r="H13" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y13" s="75" t="s">
+      <c r="H13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y13" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="Z13" s="76"/>
-      <c r="AA13" s="76"/>
-      <c r="AB13" s="75" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC13" s="76"/>
-      <c r="AD13" s="76"/>
-      <c r="AE13" s="76"/>
+      <c r="Z13" s="85"/>
+      <c r="AA13" s="85"/>
+      <c r="AB13" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC13" s="85"/>
+      <c r="AD13" s="85"/>
+      <c r="AE13" s="85"/>
     </row>
     <row r="14" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
@@ -2018,26 +2048,26 @@
       <c r="D14" s="10"/>
       <c r="E14" s="8"/>
       <c r="F14" s="3"/>
-      <c r="H14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y14" s="69" t="s">
+      <c r="H14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y14" s="78" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z14" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA14" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="Z14" s="71" t="s">
+      <c r="AB14" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="AA14" s="73" t="s">
+      <c r="AC14" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="AB14" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC14" s="62" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD14" s="63"/>
-      <c r="AE14" s="64"/>
+      <c r="AD14" s="72"/>
+      <c r="AE14" s="73"/>
     </row>
     <row r="15" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
@@ -2047,29 +2077,29 @@
       <c r="E15" s="8"/>
       <c r="F15" s="3"/>
       <c r="H15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y15" s="70"/>
-      <c r="Z15" s="72"/>
-      <c r="AA15" s="74"/>
-      <c r="AB15" s="68"/>
+        <v>21</v>
+      </c>
+      <c r="Y15" s="79"/>
+      <c r="Z15" s="81"/>
+      <c r="AA15" s="83"/>
+      <c r="AB15" s="77"/>
       <c r="AC15" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD15" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE15" s="35" t="s">
         <v>59</v>
-      </c>
-      <c r="AD15" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE15" s="35" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="21">
         <v>12</v>
@@ -2079,7 +2109,7 @@
       </c>
       <c r="F16" s="3"/>
       <c r="H16" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="Y16" s="38" t="s">
         <v>3</v>
@@ -2090,18 +2120,18 @@
       <c r="AC16" s="41"/>
       <c r="AD16" s="42"/>
       <c r="AE16" s="43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="8"/>
       <c r="F17" s="3"/>
-      <c r="H17" s="16" t="s">
-        <v>44</v>
+      <c r="H17" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="Y17" s="44"/>
       <c r="Z17" s="45" t="s">
@@ -2116,18 +2146,18 @@
       </c>
       <c r="AD17" s="48"/>
       <c r="AE17" s="49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="8"/>
       <c r="F18" s="3"/>
-      <c r="H18" s="17" t="s">
-        <v>46</v>
+      <c r="H18" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="Y18" s="44"/>
       <c r="Z18" s="45" t="s">
@@ -2143,19 +2173,22 @@
         <v>3</v>
       </c>
       <c r="AD18" s="48" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AE18" s="49" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="8"/>
       <c r="F19" s="3"/>
+      <c r="H19" s="17" t="s">
+        <v>44</v>
+      </c>
       <c r="Y19" s="50" t="s">
         <v>3</v>
       </c>
@@ -2171,7 +2204,7 @@
       </c>
       <c r="AD19" s="54"/>
       <c r="AE19" s="55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2181,9 +2214,6 @@
       <c r="D20" s="10"/>
       <c r="E20" s="8"/>
       <c r="F20" s="3"/>
-      <c r="H20" s="29" t="s">
-        <v>35</v>
-      </c>
       <c r="Y20" s="56" t="s">
         <v>3</v>
       </c>
@@ -2200,24 +2230,24 @@
         <v>3</v>
       </c>
       <c r="AD20" s="60" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AE20" s="61" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="8"/>
       <c r="F21" s="3"/>
-      <c r="H21" s="1" t="s">
-        <v>36</v>
+      <c r="H21" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="Y21" s="37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z21" s="37"/>
       <c r="AA21" s="37"/>
@@ -2234,7 +2264,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="3"/>
       <c r="H22" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.35">
@@ -2245,7 +2275,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="3"/>
       <c r="H23" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.35">
@@ -2256,10 +2286,10 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="H24" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2267,45 +2297,45 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="H25" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H26" s="31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H26" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="23" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="25"/>
-      <c r="H27" s="1" t="s">
-        <v>47</v>
+      <c r="H27" s="31" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
       <c r="H28" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>39</v>
@@ -2313,63 +2343,68 @@
     </row>
     <row r="31" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H32" s="17"/>
-    </row>
-    <row r="33" spans="2:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="34" spans="2:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H34" s="29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="H35" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="2:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="35" spans="2:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H35" s="29" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H36" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="38" spans="2:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H38" s="29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="H39" s="1" t="s">
-        <v>70</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="39" spans="2:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H39" s="29" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H40" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H41" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2402,22 +2437,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="84"/>
-    <col min="2" max="5" width="22.1796875" style="84" customWidth="1"/>
-    <col min="6" max="7" width="8.7265625" style="84"/>
-    <col min="8" max="8" width="87.36328125" style="84" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="84"/>
+    <col min="1" max="1" width="8.7265625" style="62"/>
+    <col min="2" max="5" width="22.1796875" style="62" customWidth="1"/>
+    <col min="6" max="7" width="8.7265625" style="62"/>
+    <col min="8" max="8" width="87.36328125" style="62" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="62"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
+      <c r="A1" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
@@ -2428,43 +2463,43 @@
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="85" t="s">
+      <c r="B3" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="C3" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="H3" s="62" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="84" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="84" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="84" t="s">
-        <v>83</v>
+      <c r="C4" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="62" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H7" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2482,12 +2517,12 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H11" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H12" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2502,7 +2537,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H15" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2523,7 +2558,7 @@
         <v>12</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="4:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2531,7 +2566,7 @@
         <v>14</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.3">
@@ -2539,7 +2574,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updates wireframes for ManagerView
</commit_message>
<xml_diff>
--- a/Documentation/ManagerView/ManagerView.xlsx
+++ b/Documentation/ManagerView/ManagerView.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CentRes\Documentation\ManagerView\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C17E75-C20D-4BBB-8291-16D686ED1A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA76A60-9F27-4FFF-8ADF-05327AD4AF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C5EF8A08-DD46-4887-AEB9-AF506434A2C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{C5EF8A08-DD46-4887-AEB9-AF506434A2C8}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryPopularityWindow" sheetId="1" r:id="rId1"/>
     <sheet name="EmployeeRoster" sheetId="2" r:id="rId2"/>
+    <sheet name="NewEditEmployee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="117">
   <si>
     <t>Menu Item</t>
   </si>
@@ -333,42 +334,6 @@
     <t>toggleSortKey("myTableId", "MenuCategories.name");  //toggle rotates through unsorted, sorted ASC, sorted DESC</t>
   </si>
   <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>✓</t>
-  </si>
-  <si>
-    <t>✗</t>
-  </si>
-  <si>
-    <t>Use Grid</t>
-  </si>
-  <si>
-    <t>🗑</t>
-  </si>
-  <si>
-    <t>Each cell will have a class of "employee# lastName/firstName/username/role/password"</t>
-  </si>
-  <si>
-    <t>add pointer down event listeners for each cell</t>
-  </si>
-  <si>
-    <t>classList.add("selected") to any elements with class of "employee#"</t>
-  </si>
-  <si>
-    <t>classList.remove("hidden") from inputs</t>
-  </si>
-  <si>
-    <t>move the inputs to grid-row (HINT: grid-row = employee# + 1)</t>
-  </si>
-  <si>
-    <t>classList.remove("selected") from any elements</t>
-  </si>
-  <si>
-    <t>classList.add("hidden") to inputs</t>
-  </si>
-  <si>
     <t>lblLastName</t>
   </si>
   <si>
@@ -381,77 +346,116 @@
     <t>lblRole</t>
   </si>
   <si>
-    <t>lblPwd</t>
-  </si>
-  <si>
-    <t>txtLastName</t>
-  </si>
-  <si>
-    <t>txtFirstName</t>
-  </si>
-  <si>
-    <t>txtUserName</t>
-  </si>
-  <si>
-    <t>pwdPwd</t>
-  </si>
-  <si>
-    <t>cboRole         ▼</t>
-  </si>
-  <si>
-    <t>These are inputs</t>
-  </si>
-  <si>
-    <t>When loading, get count of managers. If you try to delete yourself or change your role level to something</t>
-  </si>
-  <si>
-    <t>other than manager, but you're the only manager… Don't allow this action</t>
-  </si>
-  <si>
-    <t>setVar("selectedEmployee", employee#);</t>
-  </si>
-  <si>
-    <t>The ✗ button wil cancel any uncommited changes and deselect the selected user:</t>
-  </si>
-  <si>
-    <t>The ✓ button will set setVar("command","commit") and updateDisplay()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The 🗑 button will setVar("command","delete") and updateDisplay()… </t>
-  </si>
-  <si>
-    <t>function will:</t>
-  </si>
-  <si>
-    <t>If you have selected the top row (new employee row), only the + and ✗ button should be visible</t>
-  </si>
-  <si>
     <t>Data is sortable like InventoryPopularityWindow</t>
   </si>
   <si>
-    <t>class="employee0 lastName"</t>
-  </si>
-  <si>
-    <t>btnCommit (will have + or ✓  depending on if you're on the top row or not), btnDelete, btnCancel</t>
-  </si>
-  <si>
     <t>Roles are retrieved from the LoginRouteTable.title, and LoginRouteTable.id</t>
   </si>
   <si>
-    <t>Don't show</t>
-  </si>
-  <si>
-    <t>these</t>
-  </si>
-  <si>
-    <t>NOTE: You'll need to store the id. You'll need it later</t>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>jdoe</t>
+  </si>
+  <si>
+    <t>asdfasdfa</t>
+  </si>
+  <si>
+    <t>When an employee is selected, setVar("selectedEmployee", [SELECTED EMPLOYEE USERNAME])</t>
+  </si>
+  <si>
+    <t>If employee is deselected…. removeVar("selectedEmployee");</t>
+  </si>
+  <si>
+    <t>USE displayTemplate.php and restrictAccess to 8 on line 10</t>
+  </si>
+  <si>
+    <t>When Edit/New buttons are pressed,  form's action is changed to "NewEditEmployee.php"</t>
+  </si>
+  <si>
+    <t>selectedEmployee variable will be passed if employee is selected.</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        [New/Edit] Employee</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Role name Goes Here ▼</t>
+  </si>
+  <si>
+    <t>Reset will clear all fields if new employee. Will repopulate original employee data if sepcified</t>
+  </si>
+  <si>
+    <t>Back will return to EmployeeRoster without any prompts</t>
+  </si>
+  <si>
+    <t>Finish will add a new employee or update employee info</t>
+  </si>
+  <si>
+    <t>****************</t>
+  </si>
+  <si>
+    <t>Passphrase</t>
+  </si>
+  <si>
+    <t>Required for new employees</t>
+  </si>
+  <si>
+    <t>Finish will submit to this page, and display any errors that occur. Don’t clear fields if errors occur and not successful</t>
+  </si>
+  <si>
+    <t>NOTE: An error may occur if username already exists if you are creating a profile</t>
+  </si>
+  <si>
+    <t>Edit and New Buttons could be combined into a single button. They do the exact same thing.</t>
+  </si>
+  <si>
+    <t>It will display "Edit" if an employee is selected. Otherwise "New" is displayed</t>
+  </si>
+  <si>
+    <t>Error Messages Here</t>
+  </si>
+  <si>
+    <t>Edit/New</t>
+  </si>
+  <si>
+    <t>Delete button should not be enabled if no employee is selected</t>
+  </si>
+  <si>
+    <t>php reverse bycrpt hash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,6 +531,24 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -578,7 +600,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1105,19 +1127,6 @@
       <right style="medium">
         <color theme="0"/>
       </right>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0"/>
-      </left>
-      <right style="medium">
-        <color theme="0"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1135,11 +1144,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1325,97 +1371,117 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1605,6 +1671,260 @@
         <a:xfrm>
           <a:off x="120650" y="6159500"/>
           <a:ext cx="4819650" cy="1841500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>423864</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69381544-87FA-481E-96A5-3F8F5BA33264}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12700" y="38100"/>
+          <a:ext cx="7034214" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>336550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290AE6BA-382F-F583-2365-DB692A2FACAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5295900" y="5930900"/>
+          <a:ext cx="1397000" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>545194</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D82AE2BA-CDE6-4466-9008-DE7813BDF2F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12700" y="88900"/>
+          <a:ext cx="6318250" cy="456294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1454150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58833B9C-B058-EA0C-7273-27F751BDD9F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2152650" y="3136900"/>
+          <a:ext cx="2165350" cy="412750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1925,7 +2245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40248B8-C55E-47FB-9F82-CD1E5B948B7E}">
   <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -1959,14 +2279,14 @@
   <sheetData>
     <row r="1" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:31" ht="31" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
     </row>
     <row r="3" spans="1:31" ht="9.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
@@ -1975,15 +2295,15 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="U3" s="66" t="s">
+      <c r="U3" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
-      <c r="X3" s="67"/>
-      <c r="Y3" s="67"/>
-      <c r="Z3" s="68"/>
-      <c r="AA3" s="68"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
+      <c r="Y3" s="84"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="85"/>
     </row>
     <row r="4" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
@@ -2080,7 +2400,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="69" t="s">
+      <c r="G9" s="86" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="32" t="s">
@@ -2108,7 +2428,7 @@
         <v>75</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="70"/>
+      <c r="G10" s="87"/>
       <c r="H10" s="62" t="s">
         <v>76</v>
       </c>
@@ -2146,15 +2466,15 @@
       <c r="J12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y12" s="74" t="s">
+      <c r="Y12" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="Z12" s="75"/>
-      <c r="AA12" s="75"/>
-      <c r="AB12" s="75"/>
-      <c r="AC12" s="75"/>
-      <c r="AD12" s="75"/>
-      <c r="AE12" s="75"/>
+      <c r="Z12" s="92"/>
+      <c r="AA12" s="92"/>
+      <c r="AB12" s="92"/>
+      <c r="AC12" s="92"/>
+      <c r="AD12" s="92"/>
+      <c r="AE12" s="92"/>
     </row>
     <row r="13" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
@@ -2172,17 +2492,17 @@
       <c r="H13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y13" s="84" t="s">
+      <c r="Y13" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="Z13" s="85"/>
-      <c r="AA13" s="85"/>
-      <c r="AB13" s="84" t="s">
+      <c r="Z13" s="102"/>
+      <c r="AA13" s="102"/>
+      <c r="AB13" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="AC13" s="85"/>
-      <c r="AD13" s="85"/>
-      <c r="AE13" s="85"/>
+      <c r="AC13" s="102"/>
+      <c r="AD13" s="102"/>
+      <c r="AE13" s="102"/>
     </row>
     <row r="14" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
@@ -2194,23 +2514,23 @@
       <c r="H14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="Y14" s="78" t="s">
+      <c r="Y14" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="Z14" s="80" t="s">
+      <c r="Z14" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="AA14" s="82" t="s">
+      <c r="AA14" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="AB14" s="76" t="s">
+      <c r="AB14" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="AC14" s="71" t="s">
+      <c r="AC14" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="AD14" s="72"/>
-      <c r="AE14" s="73"/>
+      <c r="AD14" s="89"/>
+      <c r="AE14" s="90"/>
     </row>
     <row r="15" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
@@ -2222,10 +2542,10 @@
       <c r="H15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y15" s="79"/>
-      <c r="Z15" s="81"/>
-      <c r="AA15" s="83"/>
-      <c r="AB15" s="77"/>
+      <c r="Y15" s="96"/>
+      <c r="Z15" s="98"/>
+      <c r="AA15" s="100"/>
+      <c r="AB15" s="94"/>
       <c r="AC15" s="35" t="s">
         <v>57</v>
       </c>
@@ -2572,709 +2892,630 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99EC44A5-6039-4C00-ACD7-0433014697DF}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="61" customWidth="1"/>
-    <col min="2" max="2" width="0.90625" style="61" customWidth="1"/>
-    <col min="3" max="3" width="2.81640625" style="61" customWidth="1"/>
-    <col min="4" max="4" width="1" style="61" customWidth="1"/>
-    <col min="5" max="5" width="2.81640625" style="61" customWidth="1"/>
-    <col min="6" max="6" width="0.90625" style="61" customWidth="1"/>
-    <col min="7" max="10" width="22.1796875" style="61" customWidth="1"/>
-    <col min="11" max="12" width="11.453125" style="61" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" style="61"/>
-    <col min="14" max="14" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" style="61" customWidth="1"/>
+    <col min="2" max="5" width="22.1796875" style="61" customWidth="1"/>
+    <col min="6" max="6" width="6.08984375" style="61" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="61"/>
+    <col min="8" max="8" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0.81640625" style="61" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="61"/>
+    <col min="11" max="11" width="1" style="61" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="61"/>
+    <col min="13" max="13" width="0.6328125" style="61" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="43" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="A2" s="71"/>
+      <c r="B2" s="81" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="71"/>
+      <c r="H2" s="75" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="64"/>
+      <c r="B4" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="65"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="64"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="64"/>
+      <c r="H5" s="61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="64"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="64"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="64"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="64"/>
+      <c r="H7" s="61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="64"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="64"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="64"/>
+      <c r="B9" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="64"/>
+      <c r="H9" s="61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="64"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="64"/>
+      <c r="H10" s="61" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="64"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="64"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="64"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="64"/>
+      <c r="H12" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" s="70"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="64"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="64"/>
+      <c r="I13" s="70"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="64"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="64"/>
+      <c r="H14" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="70"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="64"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="64"/>
+      <c r="H15" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="70"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="64"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="64"/>
+      <c r="I16" s="70"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="64"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="64"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="64"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="64"/>
+      <c r="H18" s="61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="64"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="64"/>
+      <c r="H19" s="61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="64"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="64"/>
+      <c r="I20" s="70"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="64"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="64"/>
+      <c r="I21" s="70"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="64"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="64"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="64"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="64"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="64"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="64"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="64"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="64"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="64"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="64"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="64"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="64"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="64"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="64"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="64"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="64"/>
+    </row>
+    <row r="30" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="64"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="64"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="64"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+    </row>
+    <row r="32" spans="1:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="64"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="73"/>
+      <c r="M32" s="73"/>
+    </row>
+    <row r="33" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="64"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="K33" s="74"/>
+      <c r="L33" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="M33" s="73"/>
+    </row>
+    <row r="34" spans="1:13" ht="4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="64"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="73"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323425F4-37CD-43F6-B717-1B88CF1978C9}">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.453125" style="61" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.6328125" style="61" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" style="61" customWidth="1"/>
+    <col min="5" max="5" width="27.26953125" style="61" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" style="61" customWidth="1"/>
+    <col min="7" max="7" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.81640625" style="61" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="0.90625" style="61" customWidth="1"/>
+    <col min="11" max="11" width="8.6328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1" style="61" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" style="61" customWidth="1"/>
+    <col min="14" max="14" width="0.6328125" style="61" customWidth="1"/>
     <col min="15" max="16384" width="8.7265625" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="88" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="88" t="s">
+    <row r="1" spans="1:14" ht="43" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="A2" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="G2" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="88" t="s">
-        <v>92</v>
-      </c>
-      <c r="J3" s="88" t="s">
-        <v>93</v>
-      </c>
-      <c r="K3" s="89" t="s">
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="64"/>
+      <c r="B4" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="L3" s="87"/>
-      <c r="N3" s="61" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="86"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="91" t="s">
+      <c r="C4" s="77"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="65"/>
+      <c r="G4" s="61" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="64"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="G5" s="61" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="64"/>
+      <c r="B6" s="79" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="64"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="64"/>
+      <c r="G6" s="61" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="64"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="G7" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="86"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="86"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="86"/>
-      <c r="N5" s="96" t="s">
+    </row>
+    <row r="8" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="64"/>
+      <c r="B8" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="64"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="64"/>
+      <c r="G8" s="70" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="64"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="G9" s="70"/>
+    </row>
+    <row r="10" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="64"/>
+      <c r="B10" s="79" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="86"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92" t="s">
+      <c r="C10" s="64"/>
+      <c r="D10" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="64"/>
+    </row>
+    <row r="11" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="64"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+    </row>
+    <row r="12" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="64"/>
+      <c r="B12" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="64"/>
+      <c r="D12" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="64"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="64"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+    </row>
+    <row r="15" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="64"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+    </row>
+    <row r="16" spans="1:14" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="64"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="74"/>
+      <c r="K16" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="L16" s="74"/>
+      <c r="M16" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="N16" s="73"/>
+    </row>
+    <row r="17" spans="1:14" ht="4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="64"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+    </row>
+    <row r="18" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="64"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+    </row>
+    <row r="19" spans="1:14" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="64"/>
+      <c r="B19" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="86"/>
-      <c r="N6" s="96" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="86"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92" t="s">
-        <v>114</v>
-      </c>
-      <c r="L7" s="86"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="86"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="86"/>
-      <c r="N8" s="61" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="95" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="86"/>
-      <c r="G9" s="93" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="93" t="s">
-        <v>96</v>
-      </c>
-      <c r="I9" s="93" t="s">
-        <v>97</v>
-      </c>
-      <c r="J9" s="93" t="s">
-        <v>99</v>
-      </c>
-      <c r="K9" s="93" t="s">
-        <v>98</v>
-      </c>
-      <c r="L9" s="86"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="86"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="86"/>
-      <c r="N10" s="61" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="86"/>
-      <c r="N11" s="61" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="86"/>
-      <c r="N12" s="97" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="86"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="92"/>
-      <c r="L13" s="86"/>
-      <c r="N13" s="97" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="86"/>
-      <c r="N14" s="97" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="86"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="86"/>
-      <c r="N15" s="97" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="86"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="86"/>
-      <c r="N16" s="97" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="86"/>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="92"/>
-      <c r="H17" s="92"/>
-      <c r="I17" s="92"/>
-      <c r="J17" s="92"/>
-      <c r="K17" s="92"/>
-      <c r="L17" s="86"/>
-    </row>
-    <row r="18" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="86"/>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="86"/>
-      <c r="N18" s="98" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="86"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="92"/>
-      <c r="H19" s="92"/>
-      <c r="I19" s="92"/>
-      <c r="J19" s="92"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="86"/>
-      <c r="N19" s="99" t="s">
-        <v>104</v>
-      </c>
+      <c r="C19" s="106"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="64"/>
+      <c r="H19" s="70"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="86"/>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="92"/>
-      <c r="L20" s="86"/>
-      <c r="N20" s="100" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="86"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="92"/>
-      <c r="H21" s="92"/>
-      <c r="I21" s="92"/>
-      <c r="J21" s="92"/>
-      <c r="K21" s="92"/>
-      <c r="L21" s="86"/>
-      <c r="N21" s="101" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="86"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="92"/>
-      <c r="H22" s="92"/>
-      <c r="I22" s="92"/>
-      <c r="J22" s="92"/>
-      <c r="K22" s="92"/>
-      <c r="L22" s="86"/>
-      <c r="N22" s="98" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="86"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="92"/>
-      <c r="H23" s="92"/>
-      <c r="I23" s="92"/>
-      <c r="J23" s="92"/>
-      <c r="K23" s="92"/>
-      <c r="L23" s="86"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="86"/>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-      <c r="L24" s="86"/>
-      <c r="N24" s="61" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="86"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="92"/>
-      <c r="I25" s="92"/>
-      <c r="J25" s="92"/>
-      <c r="K25" s="92"/>
-      <c r="L25" s="86"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="86"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="92"/>
-      <c r="H26" s="92"/>
-      <c r="I26" s="92"/>
-      <c r="J26" s="92"/>
-      <c r="K26" s="92"/>
-      <c r="L26" s="86"/>
-      <c r="N26" s="61" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="86"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="92"/>
-      <c r="H27" s="92"/>
-      <c r="I27" s="92"/>
-      <c r="J27" s="92"/>
-      <c r="K27" s="92"/>
-      <c r="L27" s="86"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="86"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="92"/>
-      <c r="H28" s="92"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="92"/>
-      <c r="L28" s="86"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="86"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="92"/>
-      <c r="H29" s="92"/>
-      <c r="I29" s="92"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="92"/>
-      <c r="L29" s="86"/>
-    </row>
-    <row r="30" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="86"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="86"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="86"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="86"/>
-      <c r="N30" s="61" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="86"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="86"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="86"/>
-      <c r="J31" s="86"/>
-      <c r="K31" s="86"/>
-      <c r="L31" s="86"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="86"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="86"/>
-      <c r="H32" s="86"/>
-      <c r="I32" s="86"/>
-      <c r="J32" s="86"/>
-      <c r="K32" s="86"/>
-      <c r="L32" s="86"/>
-      <c r="N32" s="61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="86"/>
-      <c r="B33" s="86"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="H33" s="86"/>
-      <c r="I33" s="86"/>
-      <c r="J33" s="86"/>
-      <c r="K33" s="86"/>
-      <c r="L33" s="86"/>
-      <c r="N33" s="61" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="86"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="86"/>
-      <c r="I34" s="86"/>
-      <c r="J34" s="86"/>
-      <c r="K34" s="86"/>
-      <c r="L34" s="86"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="86"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-      <c r="J35" s="86"/>
-      <c r="K35" s="86"/>
-      <c r="L35" s="86"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="86"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="86"/>
-      <c r="I36" s="86"/>
-      <c r="J36" s="86"/>
-      <c r="K36" s="86"/>
-      <c r="L36" s="86"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="86"/>
-      <c r="B37" s="86"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="86"/>
-      <c r="H37" s="86"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="86"/>
-      <c r="K37" s="86"/>
-      <c r="L37" s="86"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="86"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="86"/>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="86"/>
-      <c r="L38" s="86"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="86"/>
-      <c r="B39" s="86"/>
-      <c r="C39" s="86"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="86"/>
-      <c r="F39" s="86"/>
-      <c r="G39" s="86"/>
-      <c r="H39" s="86"/>
-      <c r="I39" s="86"/>
-      <c r="J39" s="86"/>
-      <c r="K39" s="86"/>
-      <c r="L39" s="86"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="86"/>
-      <c r="B40" s="86"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
-      <c r="E40" s="86"/>
-      <c r="F40" s="86"/>
-      <c r="G40" s="86"/>
-      <c r="H40" s="86"/>
-      <c r="I40" s="86"/>
-      <c r="J40" s="86"/>
-      <c r="K40" s="86"/>
-      <c r="L40" s="86"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="86"/>
-      <c r="B41" s="86"/>
-      <c r="C41" s="86"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="86"/>
-      <c r="G41" s="86"/>
-      <c r="H41" s="86"/>
-      <c r="I41" s="86"/>
-      <c r="J41" s="86"/>
-      <c r="K41" s="86"/>
-      <c r="L41" s="86"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="64"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="64"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Updates wireframes for ManagerView"
This reverts commit b08d513a0dc529d3925157a8b10ef7eff1c445b1.
</commit_message>
<xml_diff>
--- a/Documentation/ManagerView/ManagerView.xlsx
+++ b/Documentation/ManagerView/ManagerView.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CentRes\Documentation\ManagerView\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA76A60-9F27-4FFF-8ADF-05327AD4AF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C17E75-C20D-4BBB-8291-16D686ED1A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{C5EF8A08-DD46-4887-AEB9-AF506434A2C8}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C5EF8A08-DD46-4887-AEB9-AF506434A2C8}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryPopularityWindow" sheetId="1" r:id="rId1"/>
     <sheet name="EmployeeRoster" sheetId="2" r:id="rId2"/>
-    <sheet name="NewEditEmployee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
   <si>
     <t>Menu Item</t>
   </si>
@@ -334,6 +333,42 @@
     <t>toggleSortKey("myTableId", "MenuCategories.name");  //toggle rotates through unsorted, sorted ASC, sorted DESC</t>
   </si>
   <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>✗</t>
+  </si>
+  <si>
+    <t>Use Grid</t>
+  </si>
+  <si>
+    <t>🗑</t>
+  </si>
+  <si>
+    <t>Each cell will have a class of "employee# lastName/firstName/username/role/password"</t>
+  </si>
+  <si>
+    <t>add pointer down event listeners for each cell</t>
+  </si>
+  <si>
+    <t>classList.add("selected") to any elements with class of "employee#"</t>
+  </si>
+  <si>
+    <t>classList.remove("hidden") from inputs</t>
+  </si>
+  <si>
+    <t>move the inputs to grid-row (HINT: grid-row = employee# + 1)</t>
+  </si>
+  <si>
+    <t>classList.remove("selected") from any elements</t>
+  </si>
+  <si>
+    <t>classList.add("hidden") to inputs</t>
+  </si>
+  <si>
     <t>lblLastName</t>
   </si>
   <si>
@@ -346,116 +381,77 @@
     <t>lblRole</t>
   </si>
   <si>
+    <t>lblPwd</t>
+  </si>
+  <si>
+    <t>txtLastName</t>
+  </si>
+  <si>
+    <t>txtFirstName</t>
+  </si>
+  <si>
+    <t>txtUserName</t>
+  </si>
+  <si>
+    <t>pwdPwd</t>
+  </si>
+  <si>
+    <t>cboRole         ▼</t>
+  </si>
+  <si>
+    <t>These are inputs</t>
+  </si>
+  <si>
+    <t>When loading, get count of managers. If you try to delete yourself or change your role level to something</t>
+  </si>
+  <si>
+    <t>other than manager, but you're the only manager… Don't allow this action</t>
+  </si>
+  <si>
+    <t>setVar("selectedEmployee", employee#);</t>
+  </si>
+  <si>
+    <t>The ✗ button wil cancel any uncommited changes and deselect the selected user:</t>
+  </si>
+  <si>
+    <t>The ✓ button will set setVar("command","commit") and updateDisplay()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 🗑 button will setVar("command","delete") and updateDisplay()… </t>
+  </si>
+  <si>
+    <t>function will:</t>
+  </si>
+  <si>
+    <t>If you have selected the top row (new employee row), only the + and ✗ button should be visible</t>
+  </si>
+  <si>
     <t>Data is sortable like InventoryPopularityWindow</t>
   </si>
   <si>
+    <t>class="employee0 lastName"</t>
+  </si>
+  <si>
+    <t>btnCommit (will have + or ✓  depending on if you're on the top row or not), btnDelete, btnCancel</t>
+  </si>
+  <si>
     <t>Roles are retrieved from the LoginRouteTable.title, and LoginRouteTable.id</t>
   </si>
   <si>
-    <t>Delete</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>jdoe</t>
-  </si>
-  <si>
-    <t>asdfasdfa</t>
-  </si>
-  <si>
-    <t>When an employee is selected, setVar("selectedEmployee", [SELECTED EMPLOYEE USERNAME])</t>
-  </si>
-  <si>
-    <t>If employee is deselected…. removeVar("selectedEmployee");</t>
-  </si>
-  <si>
-    <t>USE displayTemplate.php and restrictAccess to 8 on line 10</t>
-  </si>
-  <si>
-    <t>When Edit/New buttons are pressed,  form's action is changed to "NewEditEmployee.php"</t>
-  </si>
-  <si>
-    <t>selectedEmployee variable will be passed if employee is selected.</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>Finish</t>
-  </si>
-  <si>
-    <t>Back</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        [New/Edit] Employee</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>Role name Goes Here ▼</t>
-  </si>
-  <si>
-    <t>Reset will clear all fields if new employee. Will repopulate original employee data if sepcified</t>
-  </si>
-  <si>
-    <t>Back will return to EmployeeRoster without any prompts</t>
-  </si>
-  <si>
-    <t>Finish will add a new employee or update employee info</t>
-  </si>
-  <si>
-    <t>****************</t>
-  </si>
-  <si>
-    <t>Passphrase</t>
-  </si>
-  <si>
-    <t>Required for new employees</t>
-  </si>
-  <si>
-    <t>Finish will submit to this page, and display any errors that occur. Don’t clear fields if errors occur and not successful</t>
-  </si>
-  <si>
-    <t>NOTE: An error may occur if username already exists if you are creating a profile</t>
-  </si>
-  <si>
-    <t>Edit and New Buttons could be combined into a single button. They do the exact same thing.</t>
-  </si>
-  <si>
-    <t>It will display "Edit" if an employee is selected. Otherwise "New" is displayed</t>
-  </si>
-  <si>
-    <t>Error Messages Here</t>
-  </si>
-  <si>
-    <t>Edit/New</t>
-  </si>
-  <si>
-    <t>Delete button should not be enabled if no employee is selected</t>
-  </si>
-  <si>
-    <t>php reverse bycrpt hash</t>
+    <t>Don't show</t>
+  </si>
+  <si>
+    <t>these</t>
+  </si>
+  <si>
+    <t>NOTE: You'll need to store the id. You'll need it later</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,24 +527,6 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="Helvetica"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -600,7 +578,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -1127,6 +1105,19 @@
       <right style="medium">
         <color theme="0"/>
       </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1144,48 +1135,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="0"/>
-      </right>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1371,117 +1325,97 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1671,260 +1605,6 @@
         <a:xfrm>
           <a:off x="120650" y="6159500"/>
           <a:ext cx="4819650" cy="1841500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>423864</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69381544-87FA-481E-96A5-3F8F5BA33264}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="12700" y="38100"/>
-          <a:ext cx="7034214" cy="508000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>336550</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290AE6BA-382F-F583-2365-DB692A2FACAC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5295900" y="5930900"/>
-          <a:ext cx="1397000" cy="469900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>545194</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D82AE2BA-CDE6-4466-9008-DE7813BDF2F5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="12700" y="88900"/>
-          <a:ext cx="6318250" cy="456294"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1454150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58833B9C-B058-EA0C-7273-27F751BDD9F3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2152650" y="3136900"/>
-          <a:ext cx="2165350" cy="412750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2245,7 +1925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40248B8-C55E-47FB-9F82-CD1E5B948B7E}">
   <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -2279,14 +1959,14 @@
   <sheetData>
     <row r="1" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:31" ht="31" x14ac:dyDescent="0.35">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:31" ht="9.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
@@ -2295,15 +1975,15 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="U3" s="83" t="s">
+      <c r="U3" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
-      <c r="Y3" s="84"/>
-      <c r="Z3" s="85"/>
-      <c r="AA3" s="85"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="67"/>
+      <c r="Z3" s="68"/>
+      <c r="AA3" s="68"/>
     </row>
     <row r="4" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
@@ -2400,7 +2080,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="86" t="s">
+      <c r="G9" s="69" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="32" t="s">
@@ -2428,7 +2108,7 @@
         <v>75</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="87"/>
+      <c r="G10" s="70"/>
       <c r="H10" s="62" t="s">
         <v>76</v>
       </c>
@@ -2466,15 +2146,15 @@
       <c r="J12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y12" s="91" t="s">
+      <c r="Y12" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="Z12" s="92"/>
-      <c r="AA12" s="92"/>
-      <c r="AB12" s="92"/>
-      <c r="AC12" s="92"/>
-      <c r="AD12" s="92"/>
-      <c r="AE12" s="92"/>
+      <c r="Z12" s="75"/>
+      <c r="AA12" s="75"/>
+      <c r="AB12" s="75"/>
+      <c r="AC12" s="75"/>
+      <c r="AD12" s="75"/>
+      <c r="AE12" s="75"/>
     </row>
     <row r="13" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
@@ -2492,17 +2172,17 @@
       <c r="H13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y13" s="101" t="s">
+      <c r="Y13" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="Z13" s="102"/>
-      <c r="AA13" s="102"/>
-      <c r="AB13" s="101" t="s">
+      <c r="Z13" s="85"/>
+      <c r="AA13" s="85"/>
+      <c r="AB13" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="AC13" s="102"/>
-      <c r="AD13" s="102"/>
-      <c r="AE13" s="102"/>
+      <c r="AC13" s="85"/>
+      <c r="AD13" s="85"/>
+      <c r="AE13" s="85"/>
     </row>
     <row r="14" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
@@ -2514,23 +2194,23 @@
       <c r="H14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="Y14" s="95" t="s">
+      <c r="Y14" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="Z14" s="97" t="s">
+      <c r="Z14" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="AA14" s="99" t="s">
+      <c r="AA14" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="AB14" s="93" t="s">
+      <c r="AB14" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="AC14" s="88" t="s">
+      <c r="AC14" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="AD14" s="89"/>
-      <c r="AE14" s="90"/>
+      <c r="AD14" s="72"/>
+      <c r="AE14" s="73"/>
     </row>
     <row r="15" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
@@ -2542,10 +2222,10 @@
       <c r="H15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y15" s="96"/>
-      <c r="Z15" s="98"/>
-      <c r="AA15" s="100"/>
-      <c r="AB15" s="94"/>
+      <c r="Y15" s="79"/>
+      <c r="Z15" s="81"/>
+      <c r="AA15" s="83"/>
+      <c r="AB15" s="77"/>
       <c r="AC15" s="35" t="s">
         <v>57</v>
       </c>
@@ -2892,630 +2572,709 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99EC44A5-6039-4C00-ACD7-0433014697DF}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" style="61" customWidth="1"/>
-    <col min="2" max="5" width="22.1796875" style="61" customWidth="1"/>
-    <col min="6" max="6" width="6.08984375" style="61" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="61"/>
-    <col min="8" max="8" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="0.81640625" style="61" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="61"/>
-    <col min="11" max="11" width="1" style="61" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="61"/>
-    <col min="13" max="13" width="0.6328125" style="61" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="61"/>
+    <col min="1" max="1" width="2.81640625" style="61" customWidth="1"/>
+    <col min="2" max="2" width="0.90625" style="61" customWidth="1"/>
+    <col min="3" max="3" width="2.81640625" style="61" customWidth="1"/>
+    <col min="4" max="4" width="1" style="61" customWidth="1"/>
+    <col min="5" max="5" width="2.81640625" style="61" customWidth="1"/>
+    <col min="6" max="6" width="0.90625" style="61" customWidth="1"/>
+    <col min="7" max="10" width="22.1796875" style="61" customWidth="1"/>
+    <col min="11" max="12" width="11.453125" style="61" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" style="61"/>
+    <col min="14" max="14" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
-      <c r="A2" s="71"/>
-      <c r="B2" s="81" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="A1" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="71"/>
-      <c r="H2" s="75" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="86"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="88" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="88" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="64"/>
-      <c r="B4" s="66" t="s">
+      <c r="I3" s="88" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="88" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="87"/>
+      <c r="N3" s="61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="86"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="86"/>
+      <c r="E4" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="F4" s="86"/>
+      <c r="G4" s="91" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="86"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="86"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="86"/>
+      <c r="N5" s="96" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="86"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6" s="86"/>
+      <c r="N6" s="96" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="86"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92" t="s">
+        <v>114</v>
+      </c>
+      <c r="L7" s="86"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="86"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="86"/>
+      <c r="N8" s="61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="95" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="86"/>
+      <c r="C9" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="86"/>
+      <c r="E9" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="66" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="66" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="65"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="64"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="64"/>
-      <c r="H5" s="61" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="64"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="64"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="64"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="64"/>
-      <c r="H7" s="61" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="64"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="64"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="64"/>
-      <c r="B9" s="68" t="s">
+      <c r="F9" s="86"/>
+      <c r="G9" s="93" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="93" t="s">
+        <v>96</v>
+      </c>
+      <c r="I9" s="93" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="93" t="s">
+        <v>99</v>
+      </c>
+      <c r="K9" s="93" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="86"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="86"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="92"/>
+      <c r="I10" s="92"/>
+      <c r="J10" s="92"/>
+      <c r="K10" s="92"/>
+      <c r="L10" s="86"/>
+      <c r="N10" s="61" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="86"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="86"/>
+      <c r="N11" s="61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="86"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="86"/>
+      <c r="N12" s="97" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="86"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="86"/>
+      <c r="N13" s="97" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="86"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="86"/>
+      <c r="N14" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="68" t="s">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="86"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="92"/>
+      <c r="J15" s="92"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="86"/>
+      <c r="N15" s="97" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="68" t="s">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="86"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="86"/>
+      <c r="N16" s="97" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="86"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="86"/>
+    </row>
+    <row r="18" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="86"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="86"/>
+      <c r="N18" s="98" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="86"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="92"/>
+      <c r="I19" s="92"/>
+      <c r="J19" s="92"/>
+      <c r="K19" s="92"/>
+      <c r="L19" s="86"/>
+      <c r="N19" s="99" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="86"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
+      <c r="I20" s="92"/>
+      <c r="J20" s="92"/>
+      <c r="K20" s="92"/>
+      <c r="L20" s="86"/>
+      <c r="N20" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="64"/>
-      <c r="H9" s="61" t="s">
+    </row>
+    <row r="21" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="86"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="92"/>
+      <c r="I21" s="92"/>
+      <c r="J21" s="92"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="86"/>
+      <c r="N21" s="101" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="64"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="64"/>
-      <c r="H10" s="61" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="64"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="64"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="64"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="64"/>
-      <c r="H12" s="61" t="s">
+    <row r="22" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="86"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="92"/>
+      <c r="K22" s="92"/>
+      <c r="L22" s="86"/>
+      <c r="N22" s="98" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="86"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="92"/>
+      <c r="J23" s="92"/>
+      <c r="K23" s="92"/>
+      <c r="L23" s="86"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="86"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="92"/>
+      <c r="I24" s="92"/>
+      <c r="J24" s="92"/>
+      <c r="K24" s="92"/>
+      <c r="L24" s="86"/>
+      <c r="N24" s="61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="86"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="86"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="86"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="92"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="92"/>
+      <c r="K26" s="92"/>
+      <c r="L26" s="86"/>
+      <c r="N26" s="61" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="86"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="92"/>
+      <c r="H27" s="92"/>
+      <c r="I27" s="92"/>
+      <c r="J27" s="92"/>
+      <c r="K27" s="92"/>
+      <c r="L27" s="86"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="86"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="92"/>
+      <c r="I28" s="92"/>
+      <c r="J28" s="92"/>
+      <c r="K28" s="92"/>
+      <c r="L28" s="86"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="86"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="92"/>
+      <c r="J29" s="92"/>
+      <c r="K29" s="92"/>
+      <c r="L29" s="86"/>
+    </row>
+    <row r="30" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="86"/>
+      <c r="B30" s="86"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="94"/>
+      <c r="I30" s="94"/>
+      <c r="J30" s="94"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="86"/>
+      <c r="N30" s="61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="86"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="86"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="86"/>
+      <c r="H32" s="86"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="86"/>
+      <c r="L32" s="86"/>
+      <c r="N32" s="61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="86"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="H33" s="86"/>
+      <c r="I33" s="86"/>
+      <c r="J33" s="86"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="86"/>
+      <c r="N33" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="70"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="64"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="64"/>
-      <c r="I13" s="70"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="64"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="64"/>
-      <c r="H14" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I14" s="70"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="64"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="64"/>
-      <c r="H15" s="61" t="s">
-        <v>93</v>
-      </c>
-      <c r="I15" s="70"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="64"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="64"/>
-      <c r="I16" s="70"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="64"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="64"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="64"/>
-      <c r="H18" s="61" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="64"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="64"/>
-      <c r="H19" s="61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="64"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="64"/>
-      <c r="I20" s="70"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="64"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="64"/>
-      <c r="I21" s="70"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="64"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="64"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="64"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="64"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="64"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="64"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="64"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="64"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="64"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="64"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="64"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="64"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="64"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="64"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="64"/>
-    </row>
-    <row r="30" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="64"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="64"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="64"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-    </row>
-    <row r="32" spans="1:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="64"/>
-      <c r="B32" s="64"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="I32" s="73"/>
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="73"/>
-    </row>
-    <row r="33" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="64"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="I33" s="73"/>
-      <c r="J33" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="K33" s="74"/>
-      <c r="L33" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="M33" s="73"/>
-    </row>
-    <row r="34" spans="1:13" ht="4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="64"/>
-      <c r="B34" s="64"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="73"/>
-      <c r="M34" s="73"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="86"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="86"/>
+      <c r="I34" s="86"/>
+      <c r="J34" s="86"/>
+      <c r="K34" s="86"/>
+      <c r="L34" s="86"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="86"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="86"/>
+      <c r="I35" s="86"/>
+      <c r="J35" s="86"/>
+      <c r="K35" s="86"/>
+      <c r="L35" s="86"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="86"/>
+      <c r="B36" s="86"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="86"/>
+      <c r="I36" s="86"/>
+      <c r="J36" s="86"/>
+      <c r="K36" s="86"/>
+      <c r="L36" s="86"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="86"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="86"/>
+      <c r="H37" s="86"/>
+      <c r="I37" s="86"/>
+      <c r="J37" s="86"/>
+      <c r="K37" s="86"/>
+      <c r="L37" s="86"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="86"/>
+      <c r="B38" s="86"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="86"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="86"/>
+      <c r="J38" s="86"/>
+      <c r="K38" s="86"/>
+      <c r="L38" s="86"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="86"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="86"/>
+      <c r="I39" s="86"/>
+      <c r="J39" s="86"/>
+      <c r="K39" s="86"/>
+      <c r="L39" s="86"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="86"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="86"/>
+      <c r="H40" s="86"/>
+      <c r="I40" s="86"/>
+      <c r="J40" s="86"/>
+      <c r="K40" s="86"/>
+      <c r="L40" s="86"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="86"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="86"/>
+      <c r="H41" s="86"/>
+      <c r="I41" s="86"/>
+      <c r="J41" s="86"/>
+      <c r="K41" s="86"/>
+      <c r="L41" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323425F4-37CD-43F6-B717-1B88CF1978C9}">
-  <dimension ref="A1:N22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="27.453125" style="61" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" style="61" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.6328125" style="61" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" style="61" customWidth="1"/>
-    <col min="5" max="5" width="27.26953125" style="61" customWidth="1"/>
-    <col min="6" max="6" width="7.81640625" style="61" customWidth="1"/>
-    <col min="7" max="7" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="0.81640625" style="61" customWidth="1"/>
-    <col min="9" max="9" width="9.453125" style="61" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="0.90625" style="61" customWidth="1"/>
-    <col min="11" max="11" width="8.6328125" style="61" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1" style="61" customWidth="1"/>
-    <col min="13" max="13" width="9.453125" style="61" customWidth="1"/>
-    <col min="14" max="14" width="0.6328125" style="61" customWidth="1"/>
-    <col min="15" max="16384" width="8.7265625" style="61"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="43" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
-      <c r="A2" s="81" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="G2" s="75" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="64"/>
-      <c r="B4" s="78" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="65"/>
-      <c r="G4" s="61" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="64"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="G5" s="61" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="64"/>
-      <c r="B6" s="79" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="64"/>
-      <c r="G6" s="61" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="64"/>
-      <c r="B7" s="79"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="G7" s="61" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="64"/>
-      <c r="B8" s="79" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="64"/>
-      <c r="G8" s="70" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="64"/>
-      <c r="B9" s="79"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="G9" s="70"/>
-    </row>
-    <row r="10" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="64"/>
-      <c r="B10" s="79" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="80" t="s">
-        <v>102</v>
-      </c>
-      <c r="E10" s="64"/>
-    </row>
-    <row r="11" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="64"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-    </row>
-    <row r="12" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="64"/>
-      <c r="B12" s="79" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="76" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="64" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="64"/>
-      <c r="B13" s="79"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="G13" s="61" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="64"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-    </row>
-    <row r="15" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="64"/>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
-    </row>
-    <row r="16" spans="1:14" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="64"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="J16" s="74"/>
-      <c r="K16" s="72" t="s">
-        <v>97</v>
-      </c>
-      <c r="L16" s="74"/>
-      <c r="M16" s="72" t="s">
-        <v>98</v>
-      </c>
-      <c r="N16" s="73"/>
-    </row>
-    <row r="17" spans="1:14" ht="4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="73"/>
-    </row>
-    <row r="18" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="64"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-    </row>
-    <row r="19" spans="1:14" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="64"/>
-      <c r="B19" s="105" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="106"/>
-      <c r="D19" s="107"/>
-      <c r="E19" s="64"/>
-      <c r="H19" s="70"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="64"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="64"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B19:D19"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "Updates wireframes for ManagerView""
This reverts commit bc90afc95de7ea342d535863833dad0f1d6a7394.
</commit_message>
<xml_diff>
--- a/Documentation/ManagerView/ManagerView.xlsx
+++ b/Documentation/ManagerView/ManagerView.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CentRes\Documentation\ManagerView\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C17E75-C20D-4BBB-8291-16D686ED1A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA76A60-9F27-4FFF-8ADF-05327AD4AF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C5EF8A08-DD46-4887-AEB9-AF506434A2C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{C5EF8A08-DD46-4887-AEB9-AF506434A2C8}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryPopularityWindow" sheetId="1" r:id="rId1"/>
     <sheet name="EmployeeRoster" sheetId="2" r:id="rId2"/>
+    <sheet name="NewEditEmployee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="117">
   <si>
     <t>Menu Item</t>
   </si>
@@ -333,42 +334,6 @@
     <t>toggleSortKey("myTableId", "MenuCategories.name");  //toggle rotates through unsorted, sorted ASC, sorted DESC</t>
   </si>
   <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>✓</t>
-  </si>
-  <si>
-    <t>✗</t>
-  </si>
-  <si>
-    <t>Use Grid</t>
-  </si>
-  <si>
-    <t>🗑</t>
-  </si>
-  <si>
-    <t>Each cell will have a class of "employee# lastName/firstName/username/role/password"</t>
-  </si>
-  <si>
-    <t>add pointer down event listeners for each cell</t>
-  </si>
-  <si>
-    <t>classList.add("selected") to any elements with class of "employee#"</t>
-  </si>
-  <si>
-    <t>classList.remove("hidden") from inputs</t>
-  </si>
-  <si>
-    <t>move the inputs to grid-row (HINT: grid-row = employee# + 1)</t>
-  </si>
-  <si>
-    <t>classList.remove("selected") from any elements</t>
-  </si>
-  <si>
-    <t>classList.add("hidden") to inputs</t>
-  </si>
-  <si>
     <t>lblLastName</t>
   </si>
   <si>
@@ -381,77 +346,116 @@
     <t>lblRole</t>
   </si>
   <si>
-    <t>lblPwd</t>
-  </si>
-  <si>
-    <t>txtLastName</t>
-  </si>
-  <si>
-    <t>txtFirstName</t>
-  </si>
-  <si>
-    <t>txtUserName</t>
-  </si>
-  <si>
-    <t>pwdPwd</t>
-  </si>
-  <si>
-    <t>cboRole         ▼</t>
-  </si>
-  <si>
-    <t>These are inputs</t>
-  </si>
-  <si>
-    <t>When loading, get count of managers. If you try to delete yourself or change your role level to something</t>
-  </si>
-  <si>
-    <t>other than manager, but you're the only manager… Don't allow this action</t>
-  </si>
-  <si>
-    <t>setVar("selectedEmployee", employee#);</t>
-  </si>
-  <si>
-    <t>The ✗ button wil cancel any uncommited changes and deselect the selected user:</t>
-  </si>
-  <si>
-    <t>The ✓ button will set setVar("command","commit") and updateDisplay()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The 🗑 button will setVar("command","delete") and updateDisplay()… </t>
-  </si>
-  <si>
-    <t>function will:</t>
-  </si>
-  <si>
-    <t>If you have selected the top row (new employee row), only the + and ✗ button should be visible</t>
-  </si>
-  <si>
     <t>Data is sortable like InventoryPopularityWindow</t>
   </si>
   <si>
-    <t>class="employee0 lastName"</t>
-  </si>
-  <si>
-    <t>btnCommit (will have + or ✓  depending on if you're on the top row or not), btnDelete, btnCancel</t>
-  </si>
-  <si>
     <t>Roles are retrieved from the LoginRouteTable.title, and LoginRouteTable.id</t>
   </si>
   <si>
-    <t>Don't show</t>
-  </si>
-  <si>
-    <t>these</t>
-  </si>
-  <si>
-    <t>NOTE: You'll need to store the id. You'll need it later</t>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>jdoe</t>
+  </si>
+  <si>
+    <t>asdfasdfa</t>
+  </si>
+  <si>
+    <t>When an employee is selected, setVar("selectedEmployee", [SELECTED EMPLOYEE USERNAME])</t>
+  </si>
+  <si>
+    <t>If employee is deselected…. removeVar("selectedEmployee");</t>
+  </si>
+  <si>
+    <t>USE displayTemplate.php and restrictAccess to 8 on line 10</t>
+  </si>
+  <si>
+    <t>When Edit/New buttons are pressed,  form's action is changed to "NewEditEmployee.php"</t>
+  </si>
+  <si>
+    <t>selectedEmployee variable will be passed if employee is selected.</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        [New/Edit] Employee</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Role name Goes Here ▼</t>
+  </si>
+  <si>
+    <t>Reset will clear all fields if new employee. Will repopulate original employee data if sepcified</t>
+  </si>
+  <si>
+    <t>Back will return to EmployeeRoster without any prompts</t>
+  </si>
+  <si>
+    <t>Finish will add a new employee or update employee info</t>
+  </si>
+  <si>
+    <t>****************</t>
+  </si>
+  <si>
+    <t>Passphrase</t>
+  </si>
+  <si>
+    <t>Required for new employees</t>
+  </si>
+  <si>
+    <t>Finish will submit to this page, and display any errors that occur. Don’t clear fields if errors occur and not successful</t>
+  </si>
+  <si>
+    <t>NOTE: An error may occur if username already exists if you are creating a profile</t>
+  </si>
+  <si>
+    <t>Edit and New Buttons could be combined into a single button. They do the exact same thing.</t>
+  </si>
+  <si>
+    <t>It will display "Edit" if an employee is selected. Otherwise "New" is displayed</t>
+  </si>
+  <si>
+    <t>Error Messages Here</t>
+  </si>
+  <si>
+    <t>Edit/New</t>
+  </si>
+  <si>
+    <t>Delete button should not be enabled if no employee is selected</t>
+  </si>
+  <si>
+    <t>php reverse bycrpt hash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,6 +531,24 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -578,7 +600,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1105,19 +1127,6 @@
       <right style="medium">
         <color theme="0"/>
       </right>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0"/>
-      </left>
-      <right style="medium">
-        <color theme="0"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1135,11 +1144,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1325,97 +1371,117 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1605,6 +1671,260 @@
         <a:xfrm>
           <a:off x="120650" y="6159500"/>
           <a:ext cx="4819650" cy="1841500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>423864</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69381544-87FA-481E-96A5-3F8F5BA33264}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12700" y="38100"/>
+          <a:ext cx="7034214" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>336550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290AE6BA-382F-F583-2365-DB692A2FACAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5295900" y="5930900"/>
+          <a:ext cx="1397000" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>545194</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D82AE2BA-CDE6-4466-9008-DE7813BDF2F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12700" y="88900"/>
+          <a:ext cx="6318250" cy="456294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1454150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58833B9C-B058-EA0C-7273-27F751BDD9F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2152650" y="3136900"/>
+          <a:ext cx="2165350" cy="412750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1925,7 +2245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40248B8-C55E-47FB-9F82-CD1E5B948B7E}">
   <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -1959,14 +2279,14 @@
   <sheetData>
     <row r="1" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:31" ht="31" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
     </row>
     <row r="3" spans="1:31" ht="9.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
@@ -1975,15 +2295,15 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="U3" s="66" t="s">
+      <c r="U3" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
-      <c r="X3" s="67"/>
-      <c r="Y3" s="67"/>
-      <c r="Z3" s="68"/>
-      <c r="AA3" s="68"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
+      <c r="Y3" s="84"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="85"/>
     </row>
     <row r="4" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
@@ -2080,7 +2400,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="69" t="s">
+      <c r="G9" s="86" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="32" t="s">
@@ -2108,7 +2428,7 @@
         <v>75</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="70"/>
+      <c r="G10" s="87"/>
       <c r="H10" s="62" t="s">
         <v>76</v>
       </c>
@@ -2146,15 +2466,15 @@
       <c r="J12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y12" s="74" t="s">
+      <c r="Y12" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="Z12" s="75"/>
-      <c r="AA12" s="75"/>
-      <c r="AB12" s="75"/>
-      <c r="AC12" s="75"/>
-      <c r="AD12" s="75"/>
-      <c r="AE12" s="75"/>
+      <c r="Z12" s="92"/>
+      <c r="AA12" s="92"/>
+      <c r="AB12" s="92"/>
+      <c r="AC12" s="92"/>
+      <c r="AD12" s="92"/>
+      <c r="AE12" s="92"/>
     </row>
     <row r="13" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
@@ -2172,17 +2492,17 @@
       <c r="H13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y13" s="84" t="s">
+      <c r="Y13" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="Z13" s="85"/>
-      <c r="AA13" s="85"/>
-      <c r="AB13" s="84" t="s">
+      <c r="Z13" s="102"/>
+      <c r="AA13" s="102"/>
+      <c r="AB13" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="AC13" s="85"/>
-      <c r="AD13" s="85"/>
-      <c r="AE13" s="85"/>
+      <c r="AC13" s="102"/>
+      <c r="AD13" s="102"/>
+      <c r="AE13" s="102"/>
     </row>
     <row r="14" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
@@ -2194,23 +2514,23 @@
       <c r="H14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="Y14" s="78" t="s">
+      <c r="Y14" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="Z14" s="80" t="s">
+      <c r="Z14" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="AA14" s="82" t="s">
+      <c r="AA14" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="AB14" s="76" t="s">
+      <c r="AB14" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="AC14" s="71" t="s">
+      <c r="AC14" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="AD14" s="72"/>
-      <c r="AE14" s="73"/>
+      <c r="AD14" s="89"/>
+      <c r="AE14" s="90"/>
     </row>
     <row r="15" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
@@ -2222,10 +2542,10 @@
       <c r="H15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y15" s="79"/>
-      <c r="Z15" s="81"/>
-      <c r="AA15" s="83"/>
-      <c r="AB15" s="77"/>
+      <c r="Y15" s="96"/>
+      <c r="Z15" s="98"/>
+      <c r="AA15" s="100"/>
+      <c r="AB15" s="94"/>
       <c r="AC15" s="35" t="s">
         <v>57</v>
       </c>
@@ -2572,709 +2892,630 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99EC44A5-6039-4C00-ACD7-0433014697DF}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="61" customWidth="1"/>
-    <col min="2" max="2" width="0.90625" style="61" customWidth="1"/>
-    <col min="3" max="3" width="2.81640625" style="61" customWidth="1"/>
-    <col min="4" max="4" width="1" style="61" customWidth="1"/>
-    <col min="5" max="5" width="2.81640625" style="61" customWidth="1"/>
-    <col min="6" max="6" width="0.90625" style="61" customWidth="1"/>
-    <col min="7" max="10" width="22.1796875" style="61" customWidth="1"/>
-    <col min="11" max="12" width="11.453125" style="61" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" style="61"/>
-    <col min="14" max="14" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" style="61" customWidth="1"/>
+    <col min="2" max="5" width="22.1796875" style="61" customWidth="1"/>
+    <col min="6" max="6" width="6.08984375" style="61" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="61"/>
+    <col min="8" max="8" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0.81640625" style="61" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="61"/>
+    <col min="11" max="11" width="1" style="61" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="61"/>
+    <col min="13" max="13" width="0.6328125" style="61" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="43" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="A2" s="71"/>
+      <c r="B2" s="81" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="71"/>
+      <c r="H2" s="75" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="64"/>
+      <c r="B4" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="65"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="64"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="64"/>
+      <c r="H5" s="61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="64"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="64"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="64"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="64"/>
+      <c r="H7" s="61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="64"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="64"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="64"/>
+      <c r="B9" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="64"/>
+      <c r="H9" s="61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="64"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="64"/>
+      <c r="H10" s="61" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="64"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="64"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="64"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="64"/>
+      <c r="H12" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" s="70"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="64"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="64"/>
+      <c r="I13" s="70"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="64"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="64"/>
+      <c r="H14" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="70"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="64"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="64"/>
+      <c r="H15" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="70"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="64"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="64"/>
+      <c r="I16" s="70"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="64"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="64"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="64"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="64"/>
+      <c r="H18" s="61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="64"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="64"/>
+      <c r="H19" s="61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="64"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="64"/>
+      <c r="I20" s="70"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="64"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="64"/>
+      <c r="I21" s="70"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="64"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="64"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="64"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="64"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="64"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="64"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="64"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="64"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="64"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="64"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="64"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="64"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="64"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="64"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="64"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="64"/>
+    </row>
+    <row r="30" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="64"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="64"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="64"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+    </row>
+    <row r="32" spans="1:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="64"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="73"/>
+      <c r="M32" s="73"/>
+    </row>
+    <row r="33" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="64"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="K33" s="74"/>
+      <c r="L33" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="M33" s="73"/>
+    </row>
+    <row r="34" spans="1:13" ht="4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="64"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="73"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323425F4-37CD-43F6-B717-1B88CF1978C9}">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.453125" style="61" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.6328125" style="61" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" style="61" customWidth="1"/>
+    <col min="5" max="5" width="27.26953125" style="61" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" style="61" customWidth="1"/>
+    <col min="7" max="7" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.81640625" style="61" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="0.90625" style="61" customWidth="1"/>
+    <col min="11" max="11" width="8.6328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1" style="61" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" style="61" customWidth="1"/>
+    <col min="14" max="14" width="0.6328125" style="61" customWidth="1"/>
     <col min="15" max="16384" width="8.7265625" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="88" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="88" t="s">
+    <row r="1" spans="1:14" ht="43" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="A2" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="G2" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="88" t="s">
-        <v>92</v>
-      </c>
-      <c r="J3" s="88" t="s">
-        <v>93</v>
-      </c>
-      <c r="K3" s="89" t="s">
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="64"/>
+      <c r="B4" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="L3" s="87"/>
-      <c r="N3" s="61" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="86"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="91" t="s">
+      <c r="C4" s="77"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="65"/>
+      <c r="G4" s="61" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="64"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="G5" s="61" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="64"/>
+      <c r="B6" s="79" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="64"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="64"/>
+      <c r="G6" s="61" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="64"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="G7" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="86"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="86"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="86"/>
-      <c r="N5" s="96" t="s">
+    </row>
+    <row r="8" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="64"/>
+      <c r="B8" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="64"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="64"/>
+      <c r="G8" s="70" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="64"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="G9" s="70"/>
+    </row>
+    <row r="10" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="64"/>
+      <c r="B10" s="79" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="86"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92" t="s">
+      <c r="C10" s="64"/>
+      <c r="D10" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="64"/>
+    </row>
+    <row r="11" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="64"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+    </row>
+    <row r="12" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="64"/>
+      <c r="B12" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="64"/>
+      <c r="D12" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="64"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="64"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+    </row>
+    <row r="15" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="64"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+    </row>
+    <row r="16" spans="1:14" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="64"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="74"/>
+      <c r="K16" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="L16" s="74"/>
+      <c r="M16" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="N16" s="73"/>
+    </row>
+    <row r="17" spans="1:14" ht="4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="64"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+    </row>
+    <row r="18" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="64"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+    </row>
+    <row r="19" spans="1:14" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="64"/>
+      <c r="B19" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="86"/>
-      <c r="N6" s="96" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="86"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92" t="s">
-        <v>114</v>
-      </c>
-      <c r="L7" s="86"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="86"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="86"/>
-      <c r="N8" s="61" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="95" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="86"/>
-      <c r="G9" s="93" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="93" t="s">
-        <v>96</v>
-      </c>
-      <c r="I9" s="93" t="s">
-        <v>97</v>
-      </c>
-      <c r="J9" s="93" t="s">
-        <v>99</v>
-      </c>
-      <c r="K9" s="93" t="s">
-        <v>98</v>
-      </c>
-      <c r="L9" s="86"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="86"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="86"/>
-      <c r="N10" s="61" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="86"/>
-      <c r="N11" s="61" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="86"/>
-      <c r="N12" s="97" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="86"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="92"/>
-      <c r="L13" s="86"/>
-      <c r="N13" s="97" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="86"/>
-      <c r="N14" s="97" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="86"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="86"/>
-      <c r="N15" s="97" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="86"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="86"/>
-      <c r="N16" s="97" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="86"/>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="92"/>
-      <c r="H17" s="92"/>
-      <c r="I17" s="92"/>
-      <c r="J17" s="92"/>
-      <c r="K17" s="92"/>
-      <c r="L17" s="86"/>
-    </row>
-    <row r="18" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="86"/>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="86"/>
-      <c r="N18" s="98" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="86"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="92"/>
-      <c r="H19" s="92"/>
-      <c r="I19" s="92"/>
-      <c r="J19" s="92"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="86"/>
-      <c r="N19" s="99" t="s">
-        <v>104</v>
-      </c>
+      <c r="C19" s="106"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="64"/>
+      <c r="H19" s="70"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="86"/>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="92"/>
-      <c r="L20" s="86"/>
-      <c r="N20" s="100" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="86"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="92"/>
-      <c r="H21" s="92"/>
-      <c r="I21" s="92"/>
-      <c r="J21" s="92"/>
-      <c r="K21" s="92"/>
-      <c r="L21" s="86"/>
-      <c r="N21" s="101" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="86"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="92"/>
-      <c r="H22" s="92"/>
-      <c r="I22" s="92"/>
-      <c r="J22" s="92"/>
-      <c r="K22" s="92"/>
-      <c r="L22" s="86"/>
-      <c r="N22" s="98" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="86"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="92"/>
-      <c r="H23" s="92"/>
-      <c r="I23" s="92"/>
-      <c r="J23" s="92"/>
-      <c r="K23" s="92"/>
-      <c r="L23" s="86"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="86"/>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-      <c r="L24" s="86"/>
-      <c r="N24" s="61" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="86"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="92"/>
-      <c r="I25" s="92"/>
-      <c r="J25" s="92"/>
-      <c r="K25" s="92"/>
-      <c r="L25" s="86"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="86"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="92"/>
-      <c r="H26" s="92"/>
-      <c r="I26" s="92"/>
-      <c r="J26" s="92"/>
-      <c r="K26" s="92"/>
-      <c r="L26" s="86"/>
-      <c r="N26" s="61" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="86"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="92"/>
-      <c r="H27" s="92"/>
-      <c r="I27" s="92"/>
-      <c r="J27" s="92"/>
-      <c r="K27" s="92"/>
-      <c r="L27" s="86"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="86"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="92"/>
-      <c r="H28" s="92"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="92"/>
-      <c r="L28" s="86"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="86"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="92"/>
-      <c r="H29" s="92"/>
-      <c r="I29" s="92"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="92"/>
-      <c r="L29" s="86"/>
-    </row>
-    <row r="30" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="86"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="86"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="86"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="86"/>
-      <c r="N30" s="61" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="86"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="86"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="86"/>
-      <c r="J31" s="86"/>
-      <c r="K31" s="86"/>
-      <c r="L31" s="86"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="86"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="86"/>
-      <c r="H32" s="86"/>
-      <c r="I32" s="86"/>
-      <c r="J32" s="86"/>
-      <c r="K32" s="86"/>
-      <c r="L32" s="86"/>
-      <c r="N32" s="61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="86"/>
-      <c r="B33" s="86"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="H33" s="86"/>
-      <c r="I33" s="86"/>
-      <c r="J33" s="86"/>
-      <c r="K33" s="86"/>
-      <c r="L33" s="86"/>
-      <c r="N33" s="61" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="86"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="86"/>
-      <c r="I34" s="86"/>
-      <c r="J34" s="86"/>
-      <c r="K34" s="86"/>
-      <c r="L34" s="86"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="86"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-      <c r="J35" s="86"/>
-      <c r="K35" s="86"/>
-      <c r="L35" s="86"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="86"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="86"/>
-      <c r="I36" s="86"/>
-      <c r="J36" s="86"/>
-      <c r="K36" s="86"/>
-      <c r="L36" s="86"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="86"/>
-      <c r="B37" s="86"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="86"/>
-      <c r="H37" s="86"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="86"/>
-      <c r="K37" s="86"/>
-      <c r="L37" s="86"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="86"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="86"/>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="86"/>
-      <c r="L38" s="86"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="86"/>
-      <c r="B39" s="86"/>
-      <c r="C39" s="86"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="86"/>
-      <c r="F39" s="86"/>
-      <c r="G39" s="86"/>
-      <c r="H39" s="86"/>
-      <c r="I39" s="86"/>
-      <c r="J39" s="86"/>
-      <c r="K39" s="86"/>
-      <c r="L39" s="86"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="86"/>
-      <c r="B40" s="86"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
-      <c r="E40" s="86"/>
-      <c r="F40" s="86"/>
-      <c r="G40" s="86"/>
-      <c r="H40" s="86"/>
-      <c r="I40" s="86"/>
-      <c r="J40" s="86"/>
-      <c r="K40" s="86"/>
-      <c r="L40" s="86"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="86"/>
-      <c r="B41" s="86"/>
-      <c r="C41" s="86"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="86"/>
-      <c r="G41" s="86"/>
-      <c r="H41" s="86"/>
-      <c r="I41" s="86"/>
-      <c r="J41" s="86"/>
-      <c r="K41" s="86"/>
-      <c r="L41" s="86"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="64"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="64"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Undo revert to ManagerView wireframe
</commit_message>
<xml_diff>
--- a/Documentation/ManagerView/ManagerView.xlsx
+++ b/Documentation/ManagerView/ManagerView.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CentRes\Documentation\ManagerView\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C17E75-C20D-4BBB-8291-16D686ED1A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA76A60-9F27-4FFF-8ADF-05327AD4AF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C5EF8A08-DD46-4887-AEB9-AF506434A2C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{C5EF8A08-DD46-4887-AEB9-AF506434A2C8}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryPopularityWindow" sheetId="1" r:id="rId1"/>
     <sheet name="EmployeeRoster" sheetId="2" r:id="rId2"/>
+    <sheet name="NewEditEmployee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="117">
   <si>
     <t>Menu Item</t>
   </si>
@@ -333,42 +334,6 @@
     <t>toggleSortKey("myTableId", "MenuCategories.name");  //toggle rotates through unsorted, sorted ASC, sorted DESC</t>
   </si>
   <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>✓</t>
-  </si>
-  <si>
-    <t>✗</t>
-  </si>
-  <si>
-    <t>Use Grid</t>
-  </si>
-  <si>
-    <t>🗑</t>
-  </si>
-  <si>
-    <t>Each cell will have a class of "employee# lastName/firstName/username/role/password"</t>
-  </si>
-  <si>
-    <t>add pointer down event listeners for each cell</t>
-  </si>
-  <si>
-    <t>classList.add("selected") to any elements with class of "employee#"</t>
-  </si>
-  <si>
-    <t>classList.remove("hidden") from inputs</t>
-  </si>
-  <si>
-    <t>move the inputs to grid-row (HINT: grid-row = employee# + 1)</t>
-  </si>
-  <si>
-    <t>classList.remove("selected") from any elements</t>
-  </si>
-  <si>
-    <t>classList.add("hidden") to inputs</t>
-  </si>
-  <si>
     <t>lblLastName</t>
   </si>
   <si>
@@ -381,77 +346,116 @@
     <t>lblRole</t>
   </si>
   <si>
-    <t>lblPwd</t>
-  </si>
-  <si>
-    <t>txtLastName</t>
-  </si>
-  <si>
-    <t>txtFirstName</t>
-  </si>
-  <si>
-    <t>txtUserName</t>
-  </si>
-  <si>
-    <t>pwdPwd</t>
-  </si>
-  <si>
-    <t>cboRole         ▼</t>
-  </si>
-  <si>
-    <t>These are inputs</t>
-  </si>
-  <si>
-    <t>When loading, get count of managers. If you try to delete yourself or change your role level to something</t>
-  </si>
-  <si>
-    <t>other than manager, but you're the only manager… Don't allow this action</t>
-  </si>
-  <si>
-    <t>setVar("selectedEmployee", employee#);</t>
-  </si>
-  <si>
-    <t>The ✗ button wil cancel any uncommited changes and deselect the selected user:</t>
-  </si>
-  <si>
-    <t>The ✓ button will set setVar("command","commit") and updateDisplay()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The 🗑 button will setVar("command","delete") and updateDisplay()… </t>
-  </si>
-  <si>
-    <t>function will:</t>
-  </si>
-  <si>
-    <t>If you have selected the top row (new employee row), only the + and ✗ button should be visible</t>
-  </si>
-  <si>
     <t>Data is sortable like InventoryPopularityWindow</t>
   </si>
   <si>
-    <t>class="employee0 lastName"</t>
-  </si>
-  <si>
-    <t>btnCommit (will have + or ✓  depending on if you're on the top row or not), btnDelete, btnCancel</t>
-  </si>
-  <si>
     <t>Roles are retrieved from the LoginRouteTable.title, and LoginRouteTable.id</t>
   </si>
   <si>
-    <t>Don't show</t>
-  </si>
-  <si>
-    <t>these</t>
-  </si>
-  <si>
-    <t>NOTE: You'll need to store the id. You'll need it later</t>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>jdoe</t>
+  </si>
+  <si>
+    <t>asdfasdfa</t>
+  </si>
+  <si>
+    <t>When an employee is selected, setVar("selectedEmployee", [SELECTED EMPLOYEE USERNAME])</t>
+  </si>
+  <si>
+    <t>If employee is deselected…. removeVar("selectedEmployee");</t>
+  </si>
+  <si>
+    <t>USE displayTemplate.php and restrictAccess to 8 on line 10</t>
+  </si>
+  <si>
+    <t>When Edit/New buttons are pressed,  form's action is changed to "NewEditEmployee.php"</t>
+  </si>
+  <si>
+    <t>selectedEmployee variable will be passed if employee is selected.</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        [New/Edit] Employee</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Role name Goes Here ▼</t>
+  </si>
+  <si>
+    <t>Reset will clear all fields if new employee. Will repopulate original employee data if sepcified</t>
+  </si>
+  <si>
+    <t>Back will return to EmployeeRoster without any prompts</t>
+  </si>
+  <si>
+    <t>Finish will add a new employee or update employee info</t>
+  </si>
+  <si>
+    <t>****************</t>
+  </si>
+  <si>
+    <t>Passphrase</t>
+  </si>
+  <si>
+    <t>Required for new employees</t>
+  </si>
+  <si>
+    <t>Finish will submit to this page, and display any errors that occur. Don’t clear fields if errors occur and not successful</t>
+  </si>
+  <si>
+    <t>NOTE: An error may occur if username already exists if you are creating a profile</t>
+  </si>
+  <si>
+    <t>Edit and New Buttons could be combined into a single button. They do the exact same thing.</t>
+  </si>
+  <si>
+    <t>It will display "Edit" if an employee is selected. Otherwise "New" is displayed</t>
+  </si>
+  <si>
+    <t>Error Messages Here</t>
+  </si>
+  <si>
+    <t>Edit/New</t>
+  </si>
+  <si>
+    <t>Delete button should not be enabled if no employee is selected</t>
+  </si>
+  <si>
+    <t>php reverse bycrpt hash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,6 +531,24 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -578,7 +600,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1105,19 +1127,6 @@
       <right style="medium">
         <color theme="0"/>
       </right>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0"/>
-      </left>
-      <right style="medium">
-        <color theme="0"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1135,11 +1144,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1325,97 +1371,117 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1605,6 +1671,260 @@
         <a:xfrm>
           <a:off x="120650" y="6159500"/>
           <a:ext cx="4819650" cy="1841500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>423864</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69381544-87FA-481E-96A5-3F8F5BA33264}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12700" y="38100"/>
+          <a:ext cx="7034214" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>336550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290AE6BA-382F-F583-2365-DB692A2FACAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5295900" y="5930900"/>
+          <a:ext cx="1397000" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>545194</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D82AE2BA-CDE6-4466-9008-DE7813BDF2F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12700" y="88900"/>
+          <a:ext cx="6318250" cy="456294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1454150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58833B9C-B058-EA0C-7273-27F751BDD9F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2152650" y="3136900"/>
+          <a:ext cx="2165350" cy="412750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1925,7 +2245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40248B8-C55E-47FB-9F82-CD1E5B948B7E}">
   <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -1959,14 +2279,14 @@
   <sheetData>
     <row r="1" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:31" ht="31" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
     </row>
     <row r="3" spans="1:31" ht="9.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
@@ -1975,15 +2295,15 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="U3" s="66" t="s">
+      <c r="U3" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
-      <c r="X3" s="67"/>
-      <c r="Y3" s="67"/>
-      <c r="Z3" s="68"/>
-      <c r="AA3" s="68"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
+      <c r="Y3" s="84"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="85"/>
     </row>
     <row r="4" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
@@ -2080,7 +2400,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="69" t="s">
+      <c r="G9" s="86" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="32" t="s">
@@ -2108,7 +2428,7 @@
         <v>75</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="70"/>
+      <c r="G10" s="87"/>
       <c r="H10" s="62" t="s">
         <v>76</v>
       </c>
@@ -2146,15 +2466,15 @@
       <c r="J12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y12" s="74" t="s">
+      <c r="Y12" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="Z12" s="75"/>
-      <c r="AA12" s="75"/>
-      <c r="AB12" s="75"/>
-      <c r="AC12" s="75"/>
-      <c r="AD12" s="75"/>
-      <c r="AE12" s="75"/>
+      <c r="Z12" s="92"/>
+      <c r="AA12" s="92"/>
+      <c r="AB12" s="92"/>
+      <c r="AC12" s="92"/>
+      <c r="AD12" s="92"/>
+      <c r="AE12" s="92"/>
     </row>
     <row r="13" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
@@ -2172,17 +2492,17 @@
       <c r="H13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y13" s="84" t="s">
+      <c r="Y13" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="Z13" s="85"/>
-      <c r="AA13" s="85"/>
-      <c r="AB13" s="84" t="s">
+      <c r="Z13" s="102"/>
+      <c r="AA13" s="102"/>
+      <c r="AB13" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="AC13" s="85"/>
-      <c r="AD13" s="85"/>
-      <c r="AE13" s="85"/>
+      <c r="AC13" s="102"/>
+      <c r="AD13" s="102"/>
+      <c r="AE13" s="102"/>
     </row>
     <row r="14" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
@@ -2194,23 +2514,23 @@
       <c r="H14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="Y14" s="78" t="s">
+      <c r="Y14" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="Z14" s="80" t="s">
+      <c r="Z14" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="AA14" s="82" t="s">
+      <c r="AA14" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="AB14" s="76" t="s">
+      <c r="AB14" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="AC14" s="71" t="s">
+      <c r="AC14" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="AD14" s="72"/>
-      <c r="AE14" s="73"/>
+      <c r="AD14" s="89"/>
+      <c r="AE14" s="90"/>
     </row>
     <row r="15" spans="1:31" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
@@ -2222,10 +2542,10 @@
       <c r="H15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y15" s="79"/>
-      <c r="Z15" s="81"/>
-      <c r="AA15" s="83"/>
-      <c r="AB15" s="77"/>
+      <c r="Y15" s="96"/>
+      <c r="Z15" s="98"/>
+      <c r="AA15" s="100"/>
+      <c r="AB15" s="94"/>
       <c r="AC15" s="35" t="s">
         <v>57</v>
       </c>
@@ -2572,709 +2892,630 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99EC44A5-6039-4C00-ACD7-0433014697DF}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="61" customWidth="1"/>
-    <col min="2" max="2" width="0.90625" style="61" customWidth="1"/>
-    <col min="3" max="3" width="2.81640625" style="61" customWidth="1"/>
-    <col min="4" max="4" width="1" style="61" customWidth="1"/>
-    <col min="5" max="5" width="2.81640625" style="61" customWidth="1"/>
-    <col min="6" max="6" width="0.90625" style="61" customWidth="1"/>
-    <col min="7" max="10" width="22.1796875" style="61" customWidth="1"/>
-    <col min="11" max="12" width="11.453125" style="61" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" style="61"/>
-    <col min="14" max="14" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" style="61" customWidth="1"/>
+    <col min="2" max="5" width="22.1796875" style="61" customWidth="1"/>
+    <col min="6" max="6" width="6.08984375" style="61" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="61"/>
+    <col min="8" max="8" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0.81640625" style="61" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="61"/>
+    <col min="11" max="11" width="1" style="61" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="61"/>
+    <col min="13" max="13" width="0.6328125" style="61" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="61"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="43" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="A2" s="71"/>
+      <c r="B2" s="81" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="71"/>
+      <c r="H2" s="75" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="64"/>
+      <c r="B4" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="65"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="64"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="64"/>
+      <c r="H5" s="61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="64"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="64"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="64"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="64"/>
+      <c r="H7" s="61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="64"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="64"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="64"/>
+      <c r="B9" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="64"/>
+      <c r="H9" s="61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="64"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="64"/>
+      <c r="H10" s="61" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="64"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="64"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="64"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="64"/>
+      <c r="H12" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" s="70"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="64"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="64"/>
+      <c r="I13" s="70"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="64"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="64"/>
+      <c r="H14" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="70"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="64"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="64"/>
+      <c r="H15" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="70"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="64"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="64"/>
+      <c r="I16" s="70"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="64"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="64"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="64"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="64"/>
+      <c r="H18" s="61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="64"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="64"/>
+      <c r="H19" s="61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="64"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="64"/>
+      <c r="I20" s="70"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="64"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="64"/>
+      <c r="I21" s="70"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="64"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="64"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="64"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="64"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="64"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="64"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="64"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="64"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="64"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="64"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="64"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="64"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="64"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="64"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="64"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="64"/>
+    </row>
+    <row r="30" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="64"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="64"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="64"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+    </row>
+    <row r="32" spans="1:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="64"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="73"/>
+      <c r="M32" s="73"/>
+    </row>
+    <row r="33" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="64"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="K33" s="74"/>
+      <c r="L33" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="M33" s="73"/>
+    </row>
+    <row r="34" spans="1:13" ht="4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="64"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="73"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323425F4-37CD-43F6-B717-1B88CF1978C9}">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.453125" style="61" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" style="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.6328125" style="61" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" style="61" customWidth="1"/>
+    <col min="5" max="5" width="27.26953125" style="61" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" style="61" customWidth="1"/>
+    <col min="7" max="7" width="87.36328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.81640625" style="61" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" style="61" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="0.90625" style="61" customWidth="1"/>
+    <col min="11" max="11" width="8.6328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1" style="61" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" style="61" customWidth="1"/>
+    <col min="14" max="14" width="0.6328125" style="61" customWidth="1"/>
     <col min="15" max="16384" width="8.7265625" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="88" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="88" t="s">
+    <row r="1" spans="1:14" ht="43" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="A2" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="G2" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="88" t="s">
-        <v>92</v>
-      </c>
-      <c r="J3" s="88" t="s">
-        <v>93</v>
-      </c>
-      <c r="K3" s="89" t="s">
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="64"/>
+      <c r="B4" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="L3" s="87"/>
-      <c r="N3" s="61" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="86"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="91" t="s">
+      <c r="C4" s="77"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="65"/>
+      <c r="G4" s="61" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="64"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="G5" s="61" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="64"/>
+      <c r="B6" s="79" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="64"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="64"/>
+      <c r="G6" s="61" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="64"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="G7" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="86"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="86"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="86"/>
-      <c r="N5" s="96" t="s">
+    </row>
+    <row r="8" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="64"/>
+      <c r="B8" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="64"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="64"/>
+      <c r="G8" s="70" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="64"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="G9" s="70"/>
+    </row>
+    <row r="10" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="64"/>
+      <c r="B10" s="79" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="86"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92" t="s">
+      <c r="C10" s="64"/>
+      <c r="D10" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="64"/>
+    </row>
+    <row r="11" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="64"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+    </row>
+    <row r="12" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="64"/>
+      <c r="B12" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="64"/>
+      <c r="D12" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="64"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="64"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+    </row>
+    <row r="15" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="64"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+    </row>
+    <row r="16" spans="1:14" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="64"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="74"/>
+      <c r="K16" s="72" t="s">
+        <v>97</v>
+      </c>
+      <c r="L16" s="74"/>
+      <c r="M16" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="N16" s="73"/>
+    </row>
+    <row r="17" spans="1:14" ht="4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="64"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+    </row>
+    <row r="18" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="64"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+    </row>
+    <row r="19" spans="1:14" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="64"/>
+      <c r="B19" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="86"/>
-      <c r="N6" s="96" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="86"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92" t="s">
-        <v>114</v>
-      </c>
-      <c r="L7" s="86"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="86"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="86"/>
-      <c r="N8" s="61" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="95" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="86"/>
-      <c r="G9" s="93" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="93" t="s">
-        <v>96</v>
-      </c>
-      <c r="I9" s="93" t="s">
-        <v>97</v>
-      </c>
-      <c r="J9" s="93" t="s">
-        <v>99</v>
-      </c>
-      <c r="K9" s="93" t="s">
-        <v>98</v>
-      </c>
-      <c r="L9" s="86"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="86"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="86"/>
-      <c r="N10" s="61" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="86"/>
-      <c r="N11" s="61" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="86"/>
-      <c r="N12" s="97" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="86"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="92"/>
-      <c r="L13" s="86"/>
-      <c r="N13" s="97" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="86"/>
-      <c r="N14" s="97" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="86"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="86"/>
-      <c r="N15" s="97" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="86"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="86"/>
-      <c r="N16" s="97" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="86"/>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="92"/>
-      <c r="H17" s="92"/>
-      <c r="I17" s="92"/>
-      <c r="J17" s="92"/>
-      <c r="K17" s="92"/>
-      <c r="L17" s="86"/>
-    </row>
-    <row r="18" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="86"/>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="86"/>
-      <c r="N18" s="98" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="86"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="92"/>
-      <c r="H19" s="92"/>
-      <c r="I19" s="92"/>
-      <c r="J19" s="92"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="86"/>
-      <c r="N19" s="99" t="s">
-        <v>104</v>
-      </c>
+      <c r="C19" s="106"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="64"/>
+      <c r="H19" s="70"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="86"/>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="92"/>
-      <c r="L20" s="86"/>
-      <c r="N20" s="100" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="86"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="92"/>
-      <c r="H21" s="92"/>
-      <c r="I21" s="92"/>
-      <c r="J21" s="92"/>
-      <c r="K21" s="92"/>
-      <c r="L21" s="86"/>
-      <c r="N21" s="101" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="86"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="92"/>
-      <c r="H22" s="92"/>
-      <c r="I22" s="92"/>
-      <c r="J22" s="92"/>
-      <c r="K22" s="92"/>
-      <c r="L22" s="86"/>
-      <c r="N22" s="98" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="86"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="92"/>
-      <c r="H23" s="92"/>
-      <c r="I23" s="92"/>
-      <c r="J23" s="92"/>
-      <c r="K23" s="92"/>
-      <c r="L23" s="86"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="86"/>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-      <c r="L24" s="86"/>
-      <c r="N24" s="61" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="86"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="92"/>
-      <c r="I25" s="92"/>
-      <c r="J25" s="92"/>
-      <c r="K25" s="92"/>
-      <c r="L25" s="86"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="86"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="92"/>
-      <c r="H26" s="92"/>
-      <c r="I26" s="92"/>
-      <c r="J26" s="92"/>
-      <c r="K26" s="92"/>
-      <c r="L26" s="86"/>
-      <c r="N26" s="61" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="86"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="92"/>
-      <c r="H27" s="92"/>
-      <c r="I27" s="92"/>
-      <c r="J27" s="92"/>
-      <c r="K27" s="92"/>
-      <c r="L27" s="86"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="86"/>
-      <c r="B28" s="86"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="92"/>
-      <c r="H28" s="92"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="92"/>
-      <c r="L28" s="86"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="86"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="92"/>
-      <c r="H29" s="92"/>
-      <c r="I29" s="92"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="92"/>
-      <c r="L29" s="86"/>
-    </row>
-    <row r="30" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="86"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="86"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="86"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="86"/>
-      <c r="N30" s="61" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="86"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="86"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="86"/>
-      <c r="J31" s="86"/>
-      <c r="K31" s="86"/>
-      <c r="L31" s="86"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="86"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="86"/>
-      <c r="H32" s="86"/>
-      <c r="I32" s="86"/>
-      <c r="J32" s="86"/>
-      <c r="K32" s="86"/>
-      <c r="L32" s="86"/>
-      <c r="N32" s="61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="86"/>
-      <c r="B33" s="86"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="H33" s="86"/>
-      <c r="I33" s="86"/>
-      <c r="J33" s="86"/>
-      <c r="K33" s="86"/>
-      <c r="L33" s="86"/>
-      <c r="N33" s="61" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="86"/>
-      <c r="B34" s="86"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="86"/>
-      <c r="I34" s="86"/>
-      <c r="J34" s="86"/>
-      <c r="K34" s="86"/>
-      <c r="L34" s="86"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="86"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-      <c r="J35" s="86"/>
-      <c r="K35" s="86"/>
-      <c r="L35" s="86"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="86"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="86"/>
-      <c r="I36" s="86"/>
-      <c r="J36" s="86"/>
-      <c r="K36" s="86"/>
-      <c r="L36" s="86"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="86"/>
-      <c r="B37" s="86"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="86"/>
-      <c r="H37" s="86"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="86"/>
-      <c r="K37" s="86"/>
-      <c r="L37" s="86"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="86"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="86"/>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="86"/>
-      <c r="L38" s="86"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="86"/>
-      <c r="B39" s="86"/>
-      <c r="C39" s="86"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="86"/>
-      <c r="F39" s="86"/>
-      <c r="G39" s="86"/>
-      <c r="H39" s="86"/>
-      <c r="I39" s="86"/>
-      <c r="J39" s="86"/>
-      <c r="K39" s="86"/>
-      <c r="L39" s="86"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="86"/>
-      <c r="B40" s="86"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
-      <c r="E40" s="86"/>
-      <c r="F40" s="86"/>
-      <c r="G40" s="86"/>
-      <c r="H40" s="86"/>
-      <c r="I40" s="86"/>
-      <c r="J40" s="86"/>
-      <c r="K40" s="86"/>
-      <c r="L40" s="86"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="86"/>
-      <c r="B41" s="86"/>
-      <c r="C41" s="86"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="86"/>
-      <c r="G41" s="86"/>
-      <c r="H41" s="86"/>
-      <c r="I41" s="86"/>
-      <c r="J41" s="86"/>
-      <c r="K41" s="86"/>
-      <c r="L41" s="86"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="64"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="64"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>